<commit_message>
updated stats, added PPTX
</commit_message>
<xml_diff>
--- a/pbr_results.xlsx
+++ b/pbr_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephen/Projects/tmp/potus-battle-royale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A4050DD-4AE5-0443-9449-4DF015B6E717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6727B3-B16A-A346-95E8-8EDC30A17769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="3200" windowWidth="27240" windowHeight="16440" xr2:uid="{A490FBAB-D050-1648-93DA-DBA06CE469A0}"/>
   </bookViews>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,12 +610,12 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>0.97599999999999998</v>
+        <v>0.84399999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -627,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>2.4E-2</v>
+        <v>0.156</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -649,7 +649,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -666,7 +666,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <v>0.98399999999999999</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -709,7 +709,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>0.95199999999999996</v>
+        <v>0.99199999999999999</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>0.82799999999999996</v>
+        <v>0.26</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -743,7 +743,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>0.22</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="E13" s="1">
         <v>0</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="1">
-        <v>1.6E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -802,13 +802,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>0.94</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -819,13 +819,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>0.98399999999999999</v>
+        <v>0.88</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -836,13 +836,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>0.81200000000000006</v>
+        <v>0.78800000000000003</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -853,16 +853,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>0.52400000000000002</v>
+        <v>0.77200000000000002</v>
       </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -870,16 +870,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
       </c>
       <c r="C21" s="1">
-        <v>0.48399999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -887,13 +887,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
       </c>
       <c r="C22" s="1">
-        <v>0.16400000000000001</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -904,13 +904,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -921,10 +921,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B24" s="1">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="C24" s="1">
         <v>0</v>
@@ -938,10 +938,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -955,10 +955,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1">
-        <v>0.93600000000000005</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -972,10 +972,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B27" s="1">
-        <v>0.77600000000000002</v>
+        <v>0.996</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B28" s="1">
-        <v>0.55600000000000005</v>
+        <v>0.628</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1009,7 +1009,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="1">
-        <v>0.5</v>
+        <v>0.156</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
-        <v>0.22</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -1040,10 +1040,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1">
-        <v>2.8000000000000001E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B32" s="1">
-        <v>0.02</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -1074,10 +1074,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -1091,10 +1091,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -1108,7 +1108,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1193,7 +1193,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -1210,7 +1210,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>

</xml_diff>